<commit_message>
Added stuff so NotEnoughFoodException works
</commit_message>
<xml_diff>
--- a/misc/ProjectProgress.xlsx
+++ b/misc/ProjectProgress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sixtium\Documents\GitStuff\ENSF-409-Final-Project\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567A6E56-A5E5-4A79-9EEE-5AB4211523D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738344F2-27C7-454D-91F0-44B600378792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAFA53DB-60F3-4781-8F8E-1ACED3959C8C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DAFA53DB-60F3-4781-8F8E-1ACED3959C8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Class</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Need shortBy method</t>
   </si>
   <si>
     <t>Notes</t>
@@ -495,7 +492,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,7 +531,7 @@
         <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -748,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -767,9 +764,6 @@
       </c>
       <c r="I9" t="s">
         <v>23</v>
-      </c>
-      <c r="J9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -927,7 +921,7 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" si="0"/>
-        <v>0.53846153846153844</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="0"/>
@@ -951,7 +945,7 @@
       </c>
       <c r="I15" s="3">
         <f>AVERAGE(B15:H15)</f>
-        <v>0.21978021978021975</v>
+        <v>0.23076923076923078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>